<commit_message>
Prepare advanced swimming pool calculation
Parameter and attribute descriptions were added. Adjusted creation method for pools and some default values. Updated envelope surface table.
</commit_message>
<xml_diff>
--- a/teaser/examples/2021-08-10_Hüllflächen_Zonen_Shells_of_Zones.xlsx
+++ b/teaser/examples/2021-08-10_Hüllflächen_Zonen_Shells_of_Zones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rwthaachende-my.sharepoint.com/personal/benani_zoumba_rwth-aachen_de/Documents/EBC/Pool_Repos/TEASER/teaser/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_4A1A100B1B095E3C865B41D1FE1DDB1B75FDF3E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D218627-21E5-4905-9852-73CAC531FA32}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="11_4A1A100B1B095E3C865B41D1FE1DDB1B75FDF3E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2CFA98B7-CDB9-4CF1-B315-32CF29EE746E}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Envelope Surfaces" sheetId="1" r:id="rId1"/>
@@ -566,9 +566,6 @@
     <t>Filter type</t>
   </si>
   <si>
-    <t>Filter kombination</t>
-  </si>
-  <si>
     <t>Water type</t>
   </si>
   <si>
@@ -588,9 +585,6 @@
   </si>
   <si>
     <t>Night setback</t>
-  </si>
-  <si>
-    <t>Visitor number</t>
   </si>
   <si>
     <t>Pool covering outside operating hours</t>
@@ -678,6 +672,12 @@
   </si>
   <si>
     <t>[per day]</t>
+  </si>
+  <si>
+    <t>Filter combination</t>
+  </si>
+  <si>
+    <t>Visitor number per day</t>
   </si>
 </sst>
 </file>
@@ -2335,32 +2335,32 @@
   </sheetPr>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" style="22" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" style="23" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.88671875" style="23" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="18"/>
-    <col min="6" max="6" width="13.33203125" style="18" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" style="22" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="23" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="18"/>
+    <col min="6" max="6" width="13.28515625" style="18" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.44140625" style="18"/>
-    <col min="10" max="10" width="11.44140625" style="18" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="11.44140625" style="18"/>
-    <col min="14" max="14" width="7.6640625" style="18" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" style="18"/>
-    <col min="16" max="16" width="7.6640625" style="18" customWidth="1"/>
-    <col min="17" max="16384" width="11.44140625" style="18"/>
+    <col min="9" max="9" width="11.42578125" style="18"/>
+    <col min="10" max="10" width="11.42578125" style="18" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" style="18"/>
+    <col min="14" max="14" width="7.7109375" style="18" customWidth="1"/>
+    <col min="15" max="15" width="11.42578125" style="18"/>
+    <col min="16" max="16" width="7.7109375" style="18" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="176" t="s">
         <v>104</v>
       </c>
@@ -2381,7 +2381,7 @@
       <c r="P1" s="177"/>
       <c r="Q1" s="177"/>
     </row>
-    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="26"/>
       <c r="B2" s="17"/>
       <c r="C2" s="17"/>
@@ -2400,7 +2400,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
     </row>
-    <row r="3" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="161" t="s">
         <v>106</v>
       </c>
@@ -2437,9 +2437,9 @@
       </c>
       <c r="Q3" s="184"/>
     </row>
-    <row r="4" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="161" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B4" s="181" t="s">
         <v>112</v>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="Q4" s="181"/>
     </row>
-    <row r="5" spans="1:17" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="189" t="s">
         <v>33</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="189"/>
       <c r="B6" s="165" t="s">
         <v>9</v>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="189"/>
       <c r="B7" s="165" t="s">
         <v>10</v>
@@ -2623,7 +2623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="189"/>
       <c r="B8" s="166" t="s">
         <v>11</v>
@@ -2672,7 +2672,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="189" t="s">
         <v>12</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>6.04</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="189"/>
       <c r="B10" s="165" t="s">
         <v>9</v>
@@ -2772,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="189"/>
       <c r="B11" s="165" t="s">
         <v>10</v>
@@ -2820,7 +2820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="189"/>
       <c r="B12" s="168" t="s">
         <v>11</v>
@@ -2869,7 +2869,7 @@
         <v>8.64</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="161" t="s">
         <v>31</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>137.6</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="173" t="s">
         <v>13</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="174" t="s">
         <v>71</v>
       </c>
@@ -2978,13 +2978,13 @@
         <v>466.14960000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="175" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="171"/>
       <c r="C16" s="103">
-        <f>6.2*((C17/8.51)*0.5+8.51*0.5+8.51) + 6.2*(3.885+5.165)</f>
+        <f>6.2*((C19/8.51)*0.5+8.51*0.5+8.51) + 6.2*(3.885+5.165)</f>
         <v>225.04735957696826</v>
       </c>
       <c r="D16" s="117"/>
@@ -3017,144 +3017,144 @@
         <v>244.67410000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="174" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="169"/>
-      <c r="C17" s="90">
-        <f>29*8.5</f>
-        <v>246.5</v>
-      </c>
-      <c r="D17" s="95"/>
-      <c r="E17" s="86">
-        <f>8.5*31.5</f>
-        <v>267.75</v>
-      </c>
-      <c r="F17" s="89"/>
-      <c r="G17" s="90">
+    <row r="17" spans="1:18" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="175" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="171"/>
+      <c r="C17" s="103">
+        <v>0</v>
+      </c>
+      <c r="D17" s="117"/>
+      <c r="E17" s="103">
+        <v>0</v>
+      </c>
+      <c r="F17" s="118"/>
+      <c r="G17" s="114">
         <f>8*31.5</f>
         <v>252</v>
       </c>
-      <c r="H17" s="89"/>
-      <c r="I17" s="86">
-        <f>53*25</f>
-        <v>1325</v>
-      </c>
-      <c r="J17" s="89"/>
-      <c r="K17" s="86">
+      <c r="H17" s="118"/>
+      <c r="I17" s="103">
+        <v>0</v>
+      </c>
+      <c r="J17" s="118"/>
+      <c r="K17" s="103">
         <f>11.79+9.41</f>
         <v>21.2</v>
       </c>
       <c r="L17" s="91"/>
       <c r="M17" s="92"/>
       <c r="N17" s="91"/>
-      <c r="O17" s="92"/>
-      <c r="P17" s="93"/>
-      <c r="Q17" s="94">
-        <f>8*17.2+9.26*25</f>
-        <v>369.1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="175" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="171"/>
-      <c r="C18" s="103">
-        <v>0</v>
-      </c>
-      <c r="D18" s="117"/>
+      <c r="O17" s="100"/>
+      <c r="P17" s="119"/>
+      <c r="Q17" s="120">
+        <f>25*9.26</f>
+        <v>231.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="174" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="172"/>
+      <c r="C18" s="96">
+        <v>0</v>
+      </c>
+      <c r="D18" s="97"/>
       <c r="E18" s="103">
         <v>0</v>
       </c>
-      <c r="F18" s="118"/>
-      <c r="G18" s="114">
-        <f>8*31.5</f>
-        <v>252</v>
-      </c>
-      <c r="H18" s="118"/>
-      <c r="I18" s="103">
-        <v>0</v>
-      </c>
-      <c r="J18" s="118"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="96">
+        <v>0</v>
+      </c>
+      <c r="H18" s="98"/>
+      <c r="I18" s="114">
+        <f>9.26*25</f>
+        <v>231.5</v>
+      </c>
+      <c r="J18" s="98"/>
       <c r="K18" s="103">
         <f>11.79+9.41</f>
         <v>21.2</v>
       </c>
-      <c r="L18" s="91"/>
-      <c r="M18" s="92"/>
-      <c r="N18" s="91"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="99"/>
       <c r="O18" s="100"/>
-      <c r="P18" s="119"/>
-      <c r="Q18" s="120">
-        <f>25*9.26</f>
-        <v>231.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="69.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="P18" s="101"/>
+      <c r="Q18" s="102">
+        <v>0</v>
+      </c>
+      <c r="R18" s="138"/>
+    </row>
+    <row r="19" spans="1:18" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="174" t="s">
-        <v>69</v>
-      </c>
-      <c r="B19" s="172"/>
-      <c r="C19" s="96">
-        <v>0</v>
-      </c>
-      <c r="D19" s="97"/>
-      <c r="E19" s="103">
-        <v>0</v>
-      </c>
-      <c r="F19" s="98"/>
-      <c r="G19" s="96">
-        <v>0</v>
-      </c>
-      <c r="H19" s="98"/>
-      <c r="I19" s="114">
-        <f>9.26*25</f>
-        <v>231.5</v>
-      </c>
-      <c r="J19" s="98"/>
-      <c r="K19" s="103">
+        <v>34</v>
+      </c>
+      <c r="B19" s="169"/>
+      <c r="C19" s="90">
+        <f>29*8.5</f>
+        <v>246.5</v>
+      </c>
+      <c r="D19" s="95"/>
+      <c r="E19" s="86">
+        <f>8.5*31.5</f>
+        <v>267.75</v>
+      </c>
+      <c r="F19" s="89"/>
+      <c r="G19" s="90">
+        <f>8*31.5</f>
+        <v>252</v>
+      </c>
+      <c r="H19" s="89"/>
+      <c r="I19" s="86">
+        <f>53*25</f>
+        <v>1325</v>
+      </c>
+      <c r="J19" s="89"/>
+      <c r="K19" s="86">
         <f>11.79+9.41</f>
         <v>21.2</v>
       </c>
-      <c r="L19" s="99"/>
-      <c r="M19" s="100"/>
-      <c r="N19" s="99"/>
-      <c r="O19" s="100"/>
-      <c r="P19" s="101"/>
-      <c r="Q19" s="102">
-        <v>0</v>
-      </c>
-      <c r="R19" s="138"/>
-    </row>
-    <row r="20" spans="1:18" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L19" s="91"/>
+      <c r="M19" s="92"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="92"/>
+      <c r="P19" s="93"/>
+      <c r="Q19" s="94">
+        <f>8*17.2+9.26*25</f>
+        <v>369.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="69.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="174" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="172"/>
       <c r="C20" s="103">
-        <f>C17*6.2</f>
+        <f>C19*6.2</f>
         <v>1528.3</v>
       </c>
       <c r="D20" s="97"/>
       <c r="E20" s="103">
-        <f>E17*3.6</f>
+        <f>E19*3.6</f>
         <v>963.9</v>
       </c>
       <c r="F20" s="98"/>
       <c r="G20" s="103">
-        <f>G17*3.25</f>
+        <f>G19*3.25</f>
         <v>819</v>
       </c>
       <c r="H20" s="98"/>
       <c r="I20" s="103">
-        <f>I17*6.2</f>
+        <f>I19*6.2</f>
         <v>8215</v>
       </c>
       <c r="J20" s="98"/>
       <c r="K20" s="103">
-        <f>K17*3.25</f>
+        <f>K19*3.25</f>
         <v>68.899999999999991</v>
       </c>
       <c r="L20" s="99"/>
@@ -3168,7 +3168,7 @@
       </c>
       <c r="R20" s="138"/>
     </row>
-    <row r="21" spans="1:18" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" ht="58.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="134"/>
       <c r="B21" s="134"/>
       <c r="C21" s="24"/>
@@ -3188,7 +3188,7 @@
       <c r="Q21" s="19"/>
       <c r="R21" s="138"/>
     </row>
-    <row r="22" spans="1:18" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="136"/>
       <c r="B22" s="136"/>
       <c r="C22" s="136"/>
@@ -3208,7 +3208,7 @@
       <c r="Q22" s="24"/>
       <c r="R22" s="138"/>
     </row>
-    <row r="23" spans="1:18" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="135"/>
       <c r="C23" s="135"/>
@@ -3228,7 +3228,7 @@
       <c r="Q23" s="24"/>
       <c r="R23" s="138"/>
     </row>
-    <row r="24" spans="1:18" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="135"/>
       <c r="C24" s="135"/>
@@ -3247,7 +3247,7 @@
       <c r="P24" s="135"/>
       <c r="Q24" s="24"/>
     </row>
-    <row r="25" spans="1:18" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="135"/>
       <c r="C25" s="135"/>
@@ -3266,15 +3266,15 @@
       <c r="P25" s="135"/>
       <c r="Q25" s="24"/>
     </row>
-    <row r="26" spans="1:18" ht="43.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:18" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" ht="43.9" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:18" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R27" s="192"/>
     </row>
-    <row r="28" spans="1:18" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="R28" s="192"/>
     </row>
-    <row r="29" spans="1:18" ht="44.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:18" ht="46.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="1:18" ht="44.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:18" ht="46.9" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
     <mergeCell ref="R27:R28"/>
@@ -3328,26 +3328,26 @@
   <dimension ref="A1:U47"/>
   <sheetViews>
     <sheetView topLeftCell="C2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.44140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="16.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="33.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" style="29" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" style="145" customWidth="1"/>
-    <col min="7" max="7" width="46.88671875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="27.109375" style="37" customWidth="1"/>
-    <col min="10" max="10" width="16.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="16.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="29" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="145" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" style="1" customWidth="1"/>
+    <col min="8" max="9" width="27.140625" style="37" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" style="1" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" style="1" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="200" t="s">
         <v>30</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="16" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="16" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>15</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -3437,7 +3437,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="201" t="s">
         <v>51</v>
       </c>
@@ -3480,7 +3480,7 @@
       <c r="P4" s="158"/>
       <c r="Q4" s="158"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="199"/>
       <c r="B5" s="32"/>
       <c r="C5" s="32"/>
@@ -3515,7 +3515,7 @@
       <c r="P5" s="158"/>
       <c r="Q5" s="158"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="199"/>
       <c r="B6" s="32"/>
       <c r="C6" s="32"/>
@@ -3548,7 +3548,7 @@
       <c r="P6" s="158"/>
       <c r="Q6" s="158"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="199"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -3581,7 +3581,7 @@
       <c r="P7" s="158"/>
       <c r="Q7" s="158"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="199"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -3596,7 +3596,7 @@
       <c r="P8" s="158"/>
       <c r="Q8" s="158"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="197"/>
       <c r="B9" s="31"/>
       <c r="C9" s="31"/>
@@ -3613,7 +3613,7 @@
       <c r="P9" s="158"/>
       <c r="Q9" s="158"/>
     </row>
-    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="195" t="s">
         <v>52</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="P10" s="198"/>
       <c r="Q10" s="198"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="196"/>
       <c r="B11" s="28"/>
       <c r="C11" s="36"/>
@@ -3673,7 +3673,7 @@
       <c r="P11" s="198"/>
       <c r="Q11" s="198"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="196"/>
       <c r="B12" s="28"/>
       <c r="C12" s="36"/>
@@ -3695,7 +3695,7 @@
       <c r="P12" s="198"/>
       <c r="Q12" s="198"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="196"/>
       <c r="B13" s="28"/>
       <c r="C13" s="36"/>
@@ -3716,7 +3716,7 @@
       <c r="P13" s="198"/>
       <c r="Q13" s="198"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="196"/>
       <c r="B14" s="36"/>
       <c r="C14" s="36"/>
@@ -3737,7 +3737,7 @@
       <c r="P14" s="198"/>
       <c r="Q14" s="198"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="197"/>
       <c r="B15" s="30"/>
       <c r="C15" s="38"/>
@@ -3758,7 +3758,7 @@
       <c r="P15" s="198"/>
       <c r="Q15" s="198"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="195" t="s">
         <v>67</v>
       </c>
@@ -3802,7 +3802,7 @@
       <c r="P16" s="158"/>
       <c r="Q16" s="158"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="196"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -3838,7 +3838,7 @@
       <c r="P17" s="158"/>
       <c r="Q17" s="158"/>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="196"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -3872,7 +3872,7 @@
       <c r="P18" s="158"/>
       <c r="Q18" s="158"/>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="196"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -3906,7 +3906,7 @@
       <c r="P19" s="158"/>
       <c r="Q19" s="158"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="196"/>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
@@ -3940,7 +3940,7 @@
       <c r="P20" s="158"/>
       <c r="Q20" s="158"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="196"/>
       <c r="B21" s="10"/>
       <c r="C21" s="10"/>
@@ -3972,7 +3972,7 @@
       <c r="P21" s="158"/>
       <c r="Q21" s="158"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="195" t="s">
         <v>53</v>
       </c>
@@ -4017,7 +4017,7 @@
       <c r="P22" s="158"/>
       <c r="Q22" s="158"/>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="196"/>
       <c r="B23" s="28"/>
       <c r="C23" s="36"/>
@@ -4051,7 +4051,7 @@
       <c r="P23" s="158"/>
       <c r="Q23" s="158"/>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="196"/>
       <c r="B24" s="36"/>
       <c r="C24" s="36"/>
@@ -4081,7 +4081,7 @@
       <c r="M24" s="196"/>
       <c r="N24" s="196"/>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="196"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -4111,7 +4111,7 @@
       <c r="M25" s="196"/>
       <c r="N25" s="196"/>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="196"/>
       <c r="B26" s="36"/>
       <c r="C26" s="36"/>
@@ -4141,7 +4141,7 @@
       <c r="M26" s="196"/>
       <c r="N26" s="196"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="197"/>
       <c r="B27" s="30"/>
       <c r="C27" s="38"/>
@@ -4171,7 +4171,7 @@
       <c r="M27" s="197"/>
       <c r="N27" s="197"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="195" t="s">
         <v>77</v>
       </c>
@@ -4191,7 +4191,7 @@
       <c r="M28" s="195"/>
       <c r="N28" s="195"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="196"/>
       <c r="B29" s="59"/>
       <c r="C29" s="59"/>
@@ -4209,7 +4209,7 @@
       <c r="M29" s="196"/>
       <c r="N29" s="196"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="196"/>
       <c r="B30" s="59"/>
       <c r="C30" s="59"/>
@@ -4227,7 +4227,7 @@
       <c r="M30" s="196"/>
       <c r="N30" s="196"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="196"/>
       <c r="B31" s="59"/>
       <c r="C31" s="59"/>
@@ -4245,7 +4245,7 @@
       <c r="M31" s="196"/>
       <c r="N31" s="196"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="196"/>
       <c r="B32" s="59"/>
       <c r="C32" s="59"/>
@@ -4263,7 +4263,7 @@
       <c r="M32" s="196"/>
       <c r="N32" s="196"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="197"/>
       <c r="B33" s="61"/>
       <c r="C33" s="61"/>
@@ -4281,7 +4281,7 @@
       <c r="M33" s="197"/>
       <c r="N33" s="197"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="195" t="s">
         <v>76</v>
       </c>
@@ -4301,7 +4301,7 @@
       <c r="M34" s="195"/>
       <c r="N34" s="195"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="196"/>
       <c r="B35" s="59"/>
       <c r="C35" s="59"/>
@@ -4319,7 +4319,7 @@
       <c r="M35" s="196"/>
       <c r="N35" s="196"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="196"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -4337,7 +4337,7 @@
       <c r="M36" s="196"/>
       <c r="N36" s="196"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="196"/>
       <c r="B37" s="59"/>
       <c r="C37" s="59"/>
@@ -4355,7 +4355,7 @@
       <c r="M37" s="196"/>
       <c r="N37" s="196"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="196"/>
       <c r="B38" s="59"/>
       <c r="C38" s="59"/>
@@ -4373,7 +4373,7 @@
       <c r="M38" s="196"/>
       <c r="N38" s="196"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="197"/>
       <c r="B39" s="61"/>
       <c r="C39" s="61"/>
@@ -4391,7 +4391,7 @@
       <c r="M39" s="197"/>
       <c r="N39" s="197"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>84</v>
       </c>
@@ -4433,7 +4433,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="132" t="s">
         <v>54</v>
       </c>
@@ -4449,7 +4449,7 @@
       <c r="M41" s="53"/>
       <c r="N41" s="53"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="195" t="s">
         <v>83</v>
       </c>
@@ -4469,7 +4469,7 @@
       <c r="M42" s="195"/>
       <c r="N42" s="195"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="196"/>
       <c r="B43" s="129"/>
       <c r="C43" s="129"/>
@@ -4487,7 +4487,7 @@
       <c r="M43" s="196"/>
       <c r="N43" s="196"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="196"/>
       <c r="B44" s="129"/>
       <c r="C44" s="129"/>
@@ -4505,7 +4505,7 @@
       <c r="M44" s="196"/>
       <c r="N44" s="196"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="196"/>
       <c r="B45" s="129"/>
       <c r="C45" s="129"/>
@@ -4523,7 +4523,7 @@
       <c r="M45" s="196"/>
       <c r="N45" s="196"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="196"/>
       <c r="B46" s="129"/>
       <c r="C46" s="129"/>
@@ -4541,7 +4541,7 @@
       <c r="M46" s="196"/>
       <c r="N46" s="196"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="197"/>
       <c r="B47" s="130"/>
       <c r="C47" s="130"/>
@@ -4611,21 +4611,21 @@
   </sheetPr>
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView zoomScale="83" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" style="18" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" style="18" customWidth="1"/>
-    <col min="4" max="12" width="26.33203125" style="18" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="18" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="11.44140625" style="18"/>
+    <col min="1" max="1" width="25.7109375" style="18" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" style="18" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" style="18" customWidth="1"/>
+    <col min="4" max="12" width="26.28515625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1" s="176" t="s">
         <v>105</v>
       </c>
@@ -4646,7 +4646,7 @@
       <c r="P1" s="177"/>
       <c r="Q1" s="177"/>
     </row>
-    <row r="3" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="202" t="s">
         <v>107</v>
       </c>
@@ -4682,43 +4682,43 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="160" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B4" s="161"/>
       <c r="C4" s="34" t="s">
         <v>35</v>
       </c>
       <c r="D4" s="139" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="139" t="s">
+        <v>138</v>
+      </c>
+      <c r="F4" s="139" t="s">
         <v>139</v>
       </c>
-      <c r="E4" s="139" t="s">
+      <c r="G4" s="139" t="s">
         <v>140</v>
       </c>
-      <c r="F4" s="139" t="s">
+      <c r="H4" s="139" t="s">
         <v>141</v>
       </c>
-      <c r="G4" s="139" t="s">
+      <c r="I4" s="139" t="s">
         <v>142</v>
       </c>
-      <c r="H4" s="139" t="s">
+      <c r="J4" s="139" t="s">
         <v>143</v>
       </c>
-      <c r="I4" s="139" t="s">
+      <c r="K4" s="139" t="s">
         <v>144</v>
       </c>
-      <c r="J4" s="139" t="s">
+      <c r="L4" s="139" t="s">
         <v>145</v>
       </c>
-      <c r="K4" s="139" t="s">
-        <v>146</v>
-      </c>
-      <c r="L4" s="139" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:17" ht="50.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A5" s="160" t="s">
         <v>42</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>43</v>
       </c>
       <c r="C5" s="124">
-        <f t="shared" ref="C5:C10" si="0">SUM(D5:L5)</f>
+        <f t="shared" ref="C5:C12" si="0">SUM(D5:L5)</f>
         <v>541.5</v>
       </c>
       <c r="D5" s="122">
@@ -4759,343 +4759,343 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="159" t="s">
+    <row r="6" spans="1:17" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="160" t="s">
+        <v>121</v>
+      </c>
+      <c r="B6" s="162" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" s="124"/>
+      <c r="D6" s="40">
+        <f t="shared" ref="D6:L6" si="1">IF(D5&gt;0,D7/D5,0)</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="40">
+        <f t="shared" si="1"/>
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="H6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="40">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="133" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="160" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="162" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="124">
+        <f>SUM(D7:L7)</f>
+        <v>1000.6750000000001</v>
+      </c>
+      <c r="D7" s="123">
+        <f>D5*2.2</f>
+        <v>916.30000000000007</v>
+      </c>
+      <c r="E7" s="40">
+        <v>0</v>
+      </c>
+      <c r="F7" s="40">
+        <v>0</v>
+      </c>
+      <c r="G7" s="123">
+        <f>(10*12.5*1.35)/2</f>
+        <v>84.375</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0</v>
+      </c>
+      <c r="J7" s="40">
+        <v>0</v>
+      </c>
+      <c r="K7" s="40">
+        <v>0</v>
+      </c>
+      <c r="L7" s="40">
+        <v>0</v>
+      </c>
+      <c r="M7" s="33"/>
+    </row>
+    <row r="8" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="160" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" s="162" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="124"/>
+      <c r="D8" s="40">
+        <f>2*25+2*16.66</f>
+        <v>83.32</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0</v>
+      </c>
+      <c r="F8" s="40">
+        <v>0</v>
+      </c>
+      <c r="G8" s="40">
+        <f>2*12.5+2*10</f>
+        <v>45</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0</v>
+      </c>
+      <c r="I8" s="40">
+        <v>0</v>
+      </c>
+      <c r="J8" s="40">
+        <v>0</v>
+      </c>
+      <c r="K8" s="40">
+        <v>0</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0</v>
+      </c>
+      <c r="M8" s="33"/>
+    </row>
+    <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="159" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="162" t="s">
+      <c r="B9" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="124">
+      <c r="C9" s="124">
         <f t="shared" si="0"/>
         <v>716.32891940711272</v>
       </c>
-      <c r="D6" s="123">
+      <c r="D9" s="123">
         <f>D5+2.2*25*2+16.66*2</f>
         <v>559.82000000000005</v>
       </c>
-      <c r="E6" s="40">
-        <v>0</v>
-      </c>
-      <c r="F6" s="40">
-        <v>0</v>
-      </c>
-      <c r="G6" s="123">
+      <c r="E9" s="40">
+        <v>0</v>
+      </c>
+      <c r="F9" s="40">
+        <v>0</v>
+      </c>
+      <c r="G9" s="123">
         <f>1.35*12.5+SQRT(1.35^2+10^2)*12.5+1.35*10</f>
         <v>156.5089194071127</v>
       </c>
-      <c r="H6" s="40">
-        <v>0</v>
-      </c>
-      <c r="I6" s="40">
-        <v>0</v>
-      </c>
-      <c r="J6" s="40">
-        <v>0</v>
-      </c>
-      <c r="K6" s="40">
-        <v>0</v>
-      </c>
-      <c r="L6" s="40">
-        <v>0</v>
-      </c>
-      <c r="M6" s="113"/>
-    </row>
-    <row r="7" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="159" t="s">
+      <c r="H9" s="40">
+        <v>0</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0</v>
+      </c>
+      <c r="J9" s="40">
+        <v>0</v>
+      </c>
+      <c r="K9" s="40">
+        <v>0</v>
+      </c>
+      <c r="L9" s="40">
+        <v>0</v>
+      </c>
+      <c r="M9" s="113"/>
+    </row>
+    <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="159" t="s">
         <v>109</v>
       </c>
-      <c r="B7" s="162" t="s">
+      <c r="B10" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="124">
+      <c r="C10" s="124">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D7" s="125">
-        <v>0</v>
-      </c>
-      <c r="E7" s="40">
-        <v>0</v>
-      </c>
-      <c r="F7" s="40">
-        <v>0</v>
-      </c>
-      <c r="G7" s="123">
-        <v>0</v>
-      </c>
-      <c r="H7" s="40">
-        <v>0</v>
-      </c>
-      <c r="I7" s="40">
-        <v>0</v>
-      </c>
-      <c r="J7" s="40">
-        <v>0</v>
-      </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="159" t="s">
+      <c r="D10" s="125">
+        <v>0</v>
+      </c>
+      <c r="E10" s="40">
+        <v>0</v>
+      </c>
+      <c r="F10" s="40">
+        <v>0</v>
+      </c>
+      <c r="G10" s="123">
+        <v>0</v>
+      </c>
+      <c r="H10" s="40">
+        <v>0</v>
+      </c>
+      <c r="I10" s="40">
+        <v>0</v>
+      </c>
+      <c r="J10" s="40">
+        <v>0</v>
+      </c>
+      <c r="K10" s="40">
+        <v>0</v>
+      </c>
+      <c r="L10" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="159" t="s">
         <v>110</v>
       </c>
-      <c r="B8" s="162" t="s">
+      <c r="B11" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="124">
+      <c r="C11" s="124">
         <f t="shared" si="0"/>
         <v>299.82891940711272</v>
       </c>
-      <c r="D8" s="123">
-        <f>D7+2.2*25*2+16.66*2</f>
+      <c r="D11" s="123">
+        <f>D10+2.2*25*2+16.66*2</f>
         <v>143.32000000000002</v>
       </c>
-      <c r="E8" s="40">
-        <v>0</v>
-      </c>
-      <c r="F8" s="40">
-        <v>0</v>
-      </c>
-      <c r="G8" s="123">
+      <c r="E11" s="40">
+        <v>0</v>
+      </c>
+      <c r="F11" s="40">
+        <v>0</v>
+      </c>
+      <c r="G11" s="123">
         <f>1.35*12.5+SQRT(1.35^2+10^2)*12.5+1.35*10</f>
         <v>156.5089194071127</v>
       </c>
-      <c r="H8" s="40">
-        <v>0</v>
-      </c>
-      <c r="I8" s="40">
-        <v>0</v>
-      </c>
-      <c r="J8" s="40">
-        <v>0</v>
-      </c>
-      <c r="K8" s="40">
-        <v>0</v>
-      </c>
-      <c r="L8" s="40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="159" t="s">
+      <c r="H11" s="40">
+        <v>0</v>
+      </c>
+      <c r="I11" s="40">
+        <v>0</v>
+      </c>
+      <c r="J11" s="40">
+        <v>0</v>
+      </c>
+      <c r="K11" s="40">
+        <v>0</v>
+      </c>
+      <c r="L11" s="40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="159" t="s">
         <v>111</v>
       </c>
-      <c r="B9" s="162" t="s">
+      <c r="B12" s="162" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="124">
+      <c r="C12" s="124">
         <f t="shared" si="0"/>
         <v>21.658000000000001</v>
       </c>
-      <c r="D9" s="125">
+      <c r="D12" s="125">
         <f>0.5*16.66*2.6</f>
         <v>21.658000000000001</v>
       </c>
-      <c r="E9" s="40">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40">
-        <v>0</v>
-      </c>
-      <c r="G9" s="123">
-        <v>0</v>
-      </c>
-      <c r="H9" s="40">
-        <v>0</v>
-      </c>
-      <c r="I9" s="40">
-        <v>0</v>
-      </c>
-      <c r="J9" s="40">
-        <v>0</v>
-      </c>
-      <c r="K9" s="40">
-        <v>0</v>
-      </c>
-      <c r="L9" s="40">
-        <v>0</v>
-      </c>
-      <c r="M9" s="157" t="s">
+      <c r="E12" s="40">
+        <v>0</v>
+      </c>
+      <c r="F12" s="40">
+        <v>0</v>
+      </c>
+      <c r="G12" s="123">
+        <v>0</v>
+      </c>
+      <c r="H12" s="40">
+        <v>0</v>
+      </c>
+      <c r="I12" s="40">
+        <v>0</v>
+      </c>
+      <c r="J12" s="40">
+        <v>0</v>
+      </c>
+      <c r="K12" s="40">
+        <v>0</v>
+      </c>
+      <c r="L12" s="40">
+        <v>0</v>
+      </c>
+      <c r="M12" s="157" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="160" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="162" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="124">
-        <f t="shared" si="0"/>
-        <v>1000.6750000000001</v>
-      </c>
-      <c r="D10" s="123">
-        <f>D5*2.2</f>
-        <v>916.30000000000007</v>
-      </c>
-      <c r="E10" s="40">
-        <v>0</v>
-      </c>
-      <c r="F10" s="40">
-        <v>0</v>
-      </c>
-      <c r="G10" s="123">
-        <f>(10*12.5*1.35)/2</f>
-        <v>84.375</v>
-      </c>
-      <c r="H10" s="40">
-        <v>0</v>
-      </c>
-      <c r="I10" s="40">
-        <v>0</v>
-      </c>
-      <c r="J10" s="40">
-        <v>0</v>
-      </c>
-      <c r="K10" s="40">
-        <v>0</v>
-      </c>
-      <c r="L10" s="40">
-        <v>0</v>
-      </c>
-      <c r="M10" s="33"/>
-    </row>
-    <row r="11" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="160" t="s">
+    <row r="13" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="160" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="162" t="s">
+      <c r="B13" s="162" t="s">
         <v>78</v>
-      </c>
-      <c r="C11" s="124"/>
-      <c r="D11" s="40">
-        <v>303.14999999999998</v>
-      </c>
-      <c r="E11" s="40">
-        <v>0</v>
-      </c>
-      <c r="F11" s="40">
-        <v>0</v>
-      </c>
-      <c r="G11" s="40">
-        <v>303.14999999999998</v>
-      </c>
-      <c r="H11" s="40">
-        <v>0</v>
-      </c>
-      <c r="I11" s="40">
-        <v>0</v>
-      </c>
-      <c r="J11" s="40">
-        <v>0</v>
-      </c>
-      <c r="K11" s="40">
-        <v>0</v>
-      </c>
-      <c r="L11" s="40">
-        <v>0</v>
-      </c>
-      <c r="M11" s="33"/>
-    </row>
-    <row r="12" spans="1:17" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12" s="162" t="s">
-        <v>80</v>
-      </c>
-      <c r="C12" s="124"/>
-      <c r="D12" s="40">
-        <f>2*25+2*16.66</f>
-        <v>83.32</v>
-      </c>
-      <c r="E12" s="40">
-        <v>0</v>
-      </c>
-      <c r="F12" s="40">
-        <v>0</v>
-      </c>
-      <c r="G12" s="40">
-        <f>2*12.5+2*10</f>
-        <v>45</v>
-      </c>
-      <c r="H12" s="40">
-        <v>0</v>
-      </c>
-      <c r="I12" s="40">
-        <v>0</v>
-      </c>
-      <c r="J12" s="40">
-        <v>0</v>
-      </c>
-      <c r="K12" s="40">
-        <v>0</v>
-      </c>
-      <c r="L12" s="40">
-        <v>0</v>
-      </c>
-      <c r="M12" s="33"/>
-    </row>
-    <row r="13" spans="1:17" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="160" t="s">
-        <v>121</v>
-      </c>
-      <c r="B13" s="162" t="s">
-        <v>80</v>
       </c>
       <c r="C13" s="124"/>
       <c r="D13" s="40">
-        <f>IF(D5&gt;0,D10/D5,0)</f>
-        <v>2.2000000000000002</v>
+        <v>303.14999999999998</v>
       </c>
       <c r="E13" s="40">
-        <f t="shared" ref="E13:L13" si="1">IF(E5&gt;0,E10/E5,0)</f>
         <v>0</v>
       </c>
       <c r="F13" s="40">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="G13" s="40">
-        <f t="shared" si="1"/>
-        <v>0.67500000000000004</v>
+        <v>303.14999999999998</v>
       </c>
       <c r="H13" s="40">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I13" s="40">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="J13" s="40">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K13" s="40">
-        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L13" s="40">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="133" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="M13" s="33"/>
+    </row>
+    <row r="14" spans="1:17" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="160" t="s">
         <v>122</v>
       </c>
       <c r="B14" s="163" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C14" s="124"/>
       <c r="D14" s="137">
@@ -5126,7 +5126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="160" t="s">
         <v>123</v>
       </c>
@@ -5135,108 +5135,108 @@
       </c>
       <c r="C15" s="124"/>
       <c r="D15" s="40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G15" s="40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="K15" s="40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="L15" s="40" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="160" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
       <c r="B16" s="162" t="s">
         <v>81</v>
       </c>
       <c r="C16" s="124"/>
       <c r="D16" s="40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G16" s="40" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="J16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="K16" s="40" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L16" s="40" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="160" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B17" s="162" t="s">
         <v>81</v>
       </c>
       <c r="C17" s="124"/>
       <c r="D17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="H17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="I17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K17" s="40" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="160" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" s="162" t="s">
         <v>100</v>
@@ -5270,9 +5270,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="160" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B19" s="162"/>
       <c r="C19" s="124"/>
@@ -5305,9 +5305,9 @@
       </c>
       <c r="N19" s="138"/>
     </row>
-    <row r="20" spans="1:14" ht="69.900000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" ht="69.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="160" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" s="162" t="s">
         <v>79</v>
@@ -5342,9 +5342,9 @@
       </c>
       <c r="N20" s="138"/>
     </row>
-    <row r="21" spans="1:14" ht="58.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" ht="58.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="160" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B21" s="162" t="s">
         <v>82</v>
@@ -5379,86 +5379,86 @@
       </c>
       <c r="N21" s="138"/>
     </row>
-    <row r="22" spans="1:14" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="160" t="s">
         <v>130</v>
       </c>
       <c r="B22" s="162" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="124"/>
+      <c r="D22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="J22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="L22" s="40" t="s">
+        <v>87</v>
+      </c>
+      <c r="N22" s="138"/>
+    </row>
+    <row r="23" spans="1:14" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="160" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" s="162" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="124"/>
-      <c r="D22" s="123">
+      <c r="C23" s="124"/>
+      <c r="D23" s="123">
         <v>30</v>
       </c>
-      <c r="E22" s="123">
-        <v>0</v>
-      </c>
-      <c r="F22" s="123">
-        <v>0</v>
-      </c>
-      <c r="G22" s="123">
-        <v>0</v>
-      </c>
-      <c r="H22" s="123">
-        <v>0</v>
-      </c>
-      <c r="I22" s="123">
-        <v>0</v>
-      </c>
-      <c r="J22" s="123">
-        <v>0</v>
-      </c>
-      <c r="K22" s="123">
-        <v>0</v>
-      </c>
-      <c r="L22" s="123">
-        <v>0</v>
-      </c>
-      <c r="N22" s="138"/>
-    </row>
-    <row r="23" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="160" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="162" t="s">
-        <v>79</v>
-      </c>
-      <c r="C23" s="124"/>
-      <c r="D23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="F23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="G23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="I23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="J23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="K23" s="40" t="s">
-        <v>87</v>
-      </c>
-      <c r="L23" s="40" t="s">
-        <v>87</v>
+      <c r="E23" s="123">
+        <v>0</v>
+      </c>
+      <c r="F23" s="123">
+        <v>0</v>
+      </c>
+      <c r="G23" s="123">
+        <v>0</v>
+      </c>
+      <c r="H23" s="123">
+        <v>0</v>
+      </c>
+      <c r="I23" s="123">
+        <v>0</v>
+      </c>
+      <c r="J23" s="123">
+        <v>0</v>
+      </c>
+      <c r="K23" s="123">
+        <v>0</v>
+      </c>
+      <c r="L23" s="123">
+        <v>0</v>
       </c>
       <c r="N23" s="138"/>
     </row>
-    <row r="24" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="160" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="B24" s="163" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C24" s="124"/>
       <c r="D24" s="137">
@@ -5489,9 +5489,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="160" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B25" s="162" t="s">
         <v>79</v>
@@ -5525,9 +5525,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="160" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B26" s="162" t="s">
         <v>79</v>
@@ -5561,9 +5561,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="43.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" ht="43.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="160" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B27" s="162" t="s">
         <v>80</v>
@@ -5598,9 +5598,9 @@
       </c>
       <c r="N27" s="192"/>
     </row>
-    <row r="28" spans="1:14" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="160" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B28" s="162" t="s">
         <v>80</v>
@@ -5635,9 +5635,9 @@
       </c>
       <c r="N28" s="192"/>
     </row>
-    <row r="29" spans="1:14" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="160" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B29" s="162" t="s">
         <v>98</v>
@@ -5655,9 +5655,9 @@
       <c r="K29" s="40"/>
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" ht="46.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="160" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B30" s="162" t="s">
         <v>99</v>
@@ -5676,16 +5676,16 @@
       <c r="K30" s="40"/>
       <c r="L30" s="40"/>
     </row>
-    <row r="31" spans="1:14" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="160" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B31" s="162" t="s">
         <v>101</v>
       </c>
       <c r="C31" s="124"/>
       <c r="D31" s="40" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E31" s="40"/>
       <c r="F31" s="40"/>
@@ -5706,7 +5706,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E31:L31" xr:uid="{1FC741BF-6034-43DF-A5BD-8CE8F3AA0207}">
       <formula1>"Stahlbeton"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:L20 D23:L23 D25:L26 D18:L18" xr:uid="{74D43ED6-0CDA-4D50-83A1-A5DCADFAA3EB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D20:L20 D22:L22 D25:L26 D18:L18" xr:uid="{74D43ED6-0CDA-4D50-83A1-A5DCADFAA3EB}">
       <formula1>"true, false"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D31" xr:uid="{8B0D90CA-9FD2-4430-81FB-6CA14A72A471}">

</xml_diff>